<commit_message>
Started filling in education and experience; tried awesomecv
</commit_message>
<xml_diff>
--- a/cv-log.xlsx
+++ b/cv-log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Documents\Admin\CV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96C4CCC1-36DE-49E1-8936-30A3B235B672}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5246D69F-681C-4A3F-8DC7-C48420AC44CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="851" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="851" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="7" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="124">
   <si>
     <t>type</t>
   </si>
@@ -158,19 +158,253 @@
     <t>Details</t>
   </si>
   <si>
-    <t>PhD, Clinical Nutrition</t>
-  </si>
-  <si>
-    <t>Oslo University Hospital; University of Oslo</t>
-  </si>
-  <si>
     <t>Oslo, Norway</t>
   </si>
   <si>
-    <t>- Thesis: bla-bla-bla</t>
-  </si>
-  <si>
     <t>4/2014 - 8/2017</t>
+  </si>
+  <si>
+    <t>Date_start</t>
+  </si>
+  <si>
+    <t>Date_end</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>University education</t>
+  </si>
+  <si>
+    <t>Post graduate education</t>
+  </si>
+  <si>
+    <t>Doctoral degree (PhD)</t>
+  </si>
+  <si>
+    <t>Oslo University Hospital and University of Oslo</t>
+  </si>
+  <si>
+    <t>07/2013 - 12/2061</t>
+  </si>
+  <si>
+    <t>Authorization</t>
+  </si>
+  <si>
+    <t>Norwegian Directorate of Health, Registration Authority for Health Personnel (SAFH)</t>
+  </si>
+  <si>
+    <t>Master Thesis</t>
+  </si>
+  <si>
+    <t>08/2012 - 06/2013</t>
+  </si>
+  <si>
+    <t>University of Oslo</t>
+  </si>
+  <si>
+    <t>08/2011 - 06/2013</t>
+  </si>
+  <si>
+    <t>Master of Clinical Nutrition</t>
+  </si>
+  <si>
+    <t>08/2008 - 06/2011</t>
+  </si>
+  <si>
+    <t>Bachelor of Science</t>
+  </si>
+  <si>
+    <t>University of Oslo and University of Stellenbosch</t>
+  </si>
+  <si>
+    <t>Primary education (schooling)</t>
+  </si>
+  <si>
+    <t>Specialization in Science and General Studies</t>
+  </si>
+  <si>
+    <t>Bjørknes Private Upper Secondary School</t>
+  </si>
+  <si>
+    <t>08/2002 - 06/2005</t>
+  </si>
+  <si>
+    <t>08/2007 - 06/2008</t>
+  </si>
+  <si>
+    <t>Physical Education and Sports</t>
+  </si>
+  <si>
+    <t>Asker Upper Secondary School</t>
+  </si>
+  <si>
+    <t>Asker, Norway</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>2014 - 2017</t>
+  </si>
+  <si>
+    <t>2013 - 2061</t>
+  </si>
+  <si>
+    <t>2012 - 2013</t>
+  </si>
+  <si>
+    <t>2011 - 2013</t>
+  </si>
+  <si>
+    <t>2008 - 2011</t>
+  </si>
+  <si>
+    <t>2007 - 2008</t>
+  </si>
+  <si>
+    <t>2002 - 2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supervisors: Prof. Kirsten B. Holven (main supervisor), PhD, Prof. Kjetil Retterstøl, MD, PhD, and Prof. Leiv Ose, MD, PhD. Title of doctoral thesis: Early life cholesterol exposure in children with familial hypercholesterolemia and healthy children (approved 30.05.2017, defended 21.08.2017). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authorized Clinical Dietitian (License: 6182046). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supervisors: Christian A. Drevon (main supervisor) and Anders Kielland. Title of master thesis: Differentiation of skeletal muscle cells in culture – Experimental conditions and expression of myokines. </t>
+  </si>
+  <si>
+    <t>Oslo, Norway, and Cape Town, South Africa</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Postdoctoral researcher</t>
+  </si>
+  <si>
+    <t>07/2018 - Present</t>
+  </si>
+  <si>
+    <t>2018 - Present</t>
+  </si>
+  <si>
+    <t>Department of Nutrition, Institute of Basic Medical Sciences, University of Oslo</t>
+  </si>
+  <si>
+    <t>Researcher</t>
+  </si>
+  <si>
+    <t>09/2017 - 07/2018</t>
+  </si>
+  <si>
+    <t>2017 - 2018</t>
+  </si>
+  <si>
+    <t>07/2013 - Present</t>
+  </si>
+  <si>
+    <t>2013 - Present</t>
+  </si>
+  <si>
+    <t>Clinical Dietitian (kef)</t>
+  </si>
+  <si>
+    <t>Lommelegen (lommelegen.no), Aller Media AS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I answer questions related to related to clinical dietetics, nutrition, physical activity and health. </t>
+  </si>
+  <si>
+    <t>09/2016 - 11/2016</t>
+  </si>
+  <si>
+    <t>University Lecturer</t>
+  </si>
+  <si>
+    <t>Clinical communication skills, teaching for under-graduate students.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I had responsibility for data analysis-centered research projects. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">See Education and authorization. </t>
+  </si>
+  <si>
+    <t>University College Lecturer/Project Coordinator</t>
+  </si>
+  <si>
+    <t>Lecturer/Nutritionist</t>
+  </si>
+  <si>
+    <t>Assistant</t>
+  </si>
+  <si>
+    <t>Diver</t>
+  </si>
+  <si>
+    <t>08/2013 - 04/2014</t>
+  </si>
+  <si>
+    <t>01/2012 - 06/2013</t>
+  </si>
+  <si>
+    <t>11/2011 - 06/2013</t>
+  </si>
+  <si>
+    <t>05/2009 - 08/2012</t>
+  </si>
+  <si>
+    <t>07/2006 - 06/2007</t>
+  </si>
+  <si>
+    <t>2013 - 2014</t>
+  </si>
+  <si>
+    <t>2009 - 2012</t>
+  </si>
+  <si>
+    <t>2006 - 2007</t>
+  </si>
+  <si>
+    <t>Oslo and Akershus University College and University of Oslo</t>
+  </si>
+  <si>
+    <t>Student Welfare Organization in Oslo (SiO)</t>
+  </si>
+  <si>
+    <t>Weekly dietary counseling sessions for healthy subjects, as well as lectures about general nutrition topics.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coordination and implementation of practical aspects of a clinical nutrition research study. </t>
+  </si>
+  <si>
+    <t>The Sleep Laboratory, Lovisenberg Diakonale Sykehus (LDS)</t>
+  </si>
+  <si>
+    <t>Examination of individuals with sleep disorders (using polysomnography).</t>
+  </si>
+  <si>
+    <t>Naval Home Guard (Sjøheimevernet, SHV)</t>
+  </si>
+  <si>
+    <t>Karljohansvern, Horten, Norway</t>
+  </si>
+  <si>
+    <t>The Norwegian Navy, Haakonsvern</t>
+  </si>
+  <si>
+    <t>Bergen, Norway</t>
+  </si>
+  <si>
+    <t>Military service, diver for the Coast Guard KV Ålesund.</t>
+  </si>
+  <si>
+    <t>Diver for the SHV task force at the eastern part of Norway.</t>
+  </si>
+  <si>
+    <t>Other Positions</t>
   </si>
 </sst>
 </file>
@@ -206,9 +440,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,88 +732,596 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D3" sqref="C3:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" customWidth="1"/>
-    <col min="3" max="3" width="36.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.5546875" style="3" customWidth="1"/>
+    <col min="5" max="6" width="17.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="98.5546875" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="4">
+        <v>41730</v>
+      </c>
+      <c r="D3" s="4">
+        <v>42948</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>44</v>
+      <c r="I3" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="4">
+        <v>41456</v>
+      </c>
+      <c r="D4" s="4">
+        <v>59141</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="4">
+        <v>41122</v>
+      </c>
+      <c r="D5" s="4">
+        <v>41426</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="4">
+        <v>40756</v>
+      </c>
+      <c r="D6" s="4">
+        <v>41426</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="4">
+        <v>39661</v>
+      </c>
+      <c r="D7" s="4">
+        <v>40695</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="4">
+        <v>39295</v>
+      </c>
+      <c r="D8" s="4">
+        <v>39600</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="4">
+        <v>37469</v>
+      </c>
+      <c r="D9" s="4">
+        <v>38504</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="31.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" customWidth="1"/>
+    <col min="7" max="7" width="31" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" customWidth="1"/>
+    <col min="9" max="9" width="52.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="1">
+        <v>43282</v>
+      </c>
+      <c r="E3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="1">
+        <v>42979</v>
+      </c>
+      <c r="D4" s="1">
+        <v>43282</v>
+      </c>
+      <c r="E4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="1">
+        <v>41456</v>
+      </c>
+      <c r="E5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="4">
+        <v>41730</v>
+      </c>
+      <c r="D6" s="4">
+        <v>42948</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="1">
+        <v>42614</v>
+      </c>
+      <c r="D7" s="1">
+        <v>42675</v>
+      </c>
+      <c r="E7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7">
+        <v>2016</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="1">
+        <v>41487</v>
+      </c>
+      <c r="D8" s="1">
+        <v>41730</v>
+      </c>
+      <c r="E8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" t="s">
+        <v>108</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="1">
+        <v>40909</v>
+      </c>
+      <c r="D9" s="1">
+        <v>41426</v>
+      </c>
+      <c r="E9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="1">
+        <v>40848</v>
+      </c>
+      <c r="D10" s="1">
+        <v>41426</v>
+      </c>
+      <c r="E10" t="s">
+        <v>105</v>
+      </c>
+      <c r="F10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="1">
+        <v>39934</v>
+      </c>
+      <c r="D11" s="1">
+        <v>41122</v>
+      </c>
+      <c r="E11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" t="s">
+        <v>109</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H11" t="s">
+        <v>118</v>
+      </c>
+      <c r="I11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="1">
+        <v>38899</v>
+      </c>
+      <c r="D12" s="1">
+        <v>39234</v>
+      </c>
+      <c r="E12" t="s">
+        <v>107</v>
+      </c>
+      <c r="F12" t="s">
+        <v>110</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1108,18 +1859,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1142,14 +1893,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8B0CA3A-E88C-474E-AEE0-98F82CA8AFD9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4343284B-DAC8-4E8C-A531-8BA424A02C88}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -1164,4 +1907,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8B0CA3A-E88C-474E-AEE0-98F82CA8AFD9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>